<commit_message>
Add the encode functionality (convert the entry queries to numbers)
</commit_message>
<xml_diff>
--- a/dataset_50.xlsx
+++ b/dataset_50.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Sepah\wall_recommender\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFDB3391-61E0-4D36-93A3-70FCFA915B24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDEF8198-443B-48ED-B0B0-F537B6F0696D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20610" yWindow="3825" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,30 +27,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="26">
   <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>defensive</t>
-  </si>
-  <si>
-    <t>num_forces</t>
-  </si>
-  <si>
-    <t>visibility</t>
-  </si>
-  <si>
     <t>water_level</t>
   </si>
   <si>
-    <t>soil_type</t>
-  </si>
-  <si>
-    <t>topography</t>
-  </si>
-  <si>
-    <t>importance</t>
-  </si>
-  <si>
     <t>speed</t>
   </si>
   <si>
@@ -66,43 +45,64 @@
     <t>avg</t>
   </si>
   <si>
-    <t>n</t>
-  </si>
-  <si>
     <t>high</t>
   </si>
   <si>
     <t>low</t>
   </si>
   <si>
+    <t>weak</t>
+  </si>
+  <si>
+    <t>hill</t>
+  </si>
+  <si>
+    <t>short</t>
+  </si>
+  <si>
+    <t>difficult</t>
+  </si>
+  <si>
+    <t>defenosive</t>
+  </si>
+  <si>
+    <t>noum_forces</t>
+  </si>
+  <si>
+    <t>importanoce</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>accessibilityes</t>
+  </si>
+  <si>
+    <t>visibilityes</t>
+  </si>
+  <si>
+    <t>soil_tyespe</t>
+  </si>
+  <si>
+    <t>topographyes</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
     <t>easy</t>
   </si>
   <si>
-    <t>weak</t>
+    <t>plain</t>
+  </si>
+  <si>
+    <t>mountain</t>
+  </si>
+  <si>
+    <t>long</t>
   </si>
   <si>
     <t>strong</t>
-  </si>
-  <si>
-    <t>plain</t>
-  </si>
-  <si>
-    <t>hill</t>
-  </si>
-  <si>
-    <t>short</t>
-  </si>
-  <si>
-    <t>long</t>
-  </si>
-  <si>
-    <t>accessibility</t>
-  </si>
-  <si>
-    <t>mountain</t>
-  </si>
-  <si>
-    <t>difficult</t>
   </si>
 </sst>
 </file>
@@ -293,15 +293,15 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5469D414-C76D-475F-8DBF-B402E31C2529}" name="Table1" displayName="Table1" ref="A1:J24" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1" totalsRowBorderDxfId="0">
   <autoFilter ref="A1:J24" xr:uid="{3666685D-B581-4997-AE6C-4CA1E08DE5ED}"/>
   <tableColumns count="10">
-    <tableColumn id="2" xr3:uid="{BACC7EB3-7AB7-4287-9974-A4729ADCEF86}" name="accessibility"/>
-    <tableColumn id="3" xr3:uid="{599103BA-5FA5-434F-B4C2-0ACF492F0C9A}" name="defensive"/>
-    <tableColumn id="4" xr3:uid="{6A166077-FFCE-4F69-8125-A23B236920E0}" name="num_forces"/>
-    <tableColumn id="5" xr3:uid="{792EAE4D-93EA-49D3-989C-201A1379E960}" name="visibility"/>
+    <tableColumn id="2" xr3:uid="{BACC7EB3-7AB7-4287-9974-A4729ADCEF86}" name="accessibilityes"/>
+    <tableColumn id="3" xr3:uid="{599103BA-5FA5-434F-B4C2-0ACF492F0C9A}" name="defenosive"/>
+    <tableColumn id="4" xr3:uid="{6A166077-FFCE-4F69-8125-A23B236920E0}" name="noum_forces"/>
+    <tableColumn id="5" xr3:uid="{792EAE4D-93EA-49D3-989C-201A1379E960}" name="visibilityes"/>
     <tableColumn id="6" xr3:uid="{005B0A7E-A078-4355-BC9E-4E55CF068D02}" name="water_level"/>
-    <tableColumn id="7" xr3:uid="{D9436875-3359-4156-98A4-2BED65FECCB6}" name="soil_type"/>
-    <tableColumn id="8" xr3:uid="{A91F4A12-7467-4B66-A440-479DBD0D93AB}" name="topography"/>
+    <tableColumn id="7" xr3:uid="{D9436875-3359-4156-98A4-2BED65FECCB6}" name="soil_tyespe"/>
+    <tableColumn id="8" xr3:uid="{A91F4A12-7467-4B66-A440-479DBD0D93AB}" name="topographyes"/>
     <tableColumn id="9" xr3:uid="{FEC8AEB5-E24E-4A6C-8077-4EE5A91A778A}" name="speed"/>
-    <tableColumn id="10" xr3:uid="{472A718B-5FE1-4EDC-B18F-AC219C36C91F}" name="importance"/>
+    <tableColumn id="10" xr3:uid="{472A718B-5FE1-4EDC-B18F-AC219C36C91F}" name="importanoce"/>
     <tableColumn id="11" xr3:uid="{9415BD32-CFD5-405B-9AAF-FAE20A48A583}" name="output"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
@@ -573,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -590,65 +590,65 @@
     <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16.5" thickBot="1">
+    <row r="1" spans="1:10" ht="32.25" thickBot="1">
       <c r="A1" s="5" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="I1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickTop="1">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>18</v>
-      </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="H2" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="I2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -656,31 +656,31 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H3" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="I3" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="J3">
         <v>2</v>
@@ -688,31 +688,31 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="G4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="H4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I4" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="J4">
         <v>3</v>
@@ -720,31 +720,31 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="F5" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H5" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="I5" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -752,31 +752,31 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="G6" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H6" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="I6" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -784,31 +784,31 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="F7" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="G7" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="H7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I7" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="J7">
         <v>2</v>
@@ -816,31 +816,31 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F8" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="G8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H8" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="I8" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="J8">
         <v>3</v>
@@ -848,31 +848,31 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E9" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F9" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="G9" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H9" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="I9" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="J9">
         <v>2</v>
@@ -880,31 +880,31 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" t="s">
         <v>25</v>
       </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" t="s">
-        <v>18</v>
-      </c>
       <c r="G10" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="H10" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I10" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="J10">
         <v>3</v>
@@ -912,31 +912,31 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E11" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F11" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="G11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H11" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="I11" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="J11">
         <v>1</v>
@@ -944,31 +944,31 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" t="s">
         <v>25</v>
       </c>
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" t="s">
-        <v>18</v>
-      </c>
       <c r="G12" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="H12" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I12" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="J12">
         <v>3</v>
@@ -976,31 +976,31 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E13" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F13" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="G13" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H13" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="I13" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="J13">
         <v>1</v>
@@ -1008,31 +1008,31 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E14" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F14" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="G14" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="H14" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="I14" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="J14">
         <v>4</v>
@@ -1040,31 +1040,31 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E15" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F15" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="G15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H15" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="I15" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="J15">
         <v>1</v>
@@ -1072,31 +1072,31 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E16" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="F16" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="G16" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="H16" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="I16" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="J16">
         <v>3</v>
@@ -1104,31 +1104,31 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" t="s">
         <v>25</v>
       </c>
-      <c r="B17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" t="s">
-        <v>0</v>
-      </c>
-      <c r="E17" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17" t="s">
-        <v>18</v>
-      </c>
       <c r="G17" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="H17" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I17" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="J17">
         <v>1</v>
@@ -1136,31 +1136,31 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E18" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="F18" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="G18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H18" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="I18" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="J18">
         <v>3</v>
@@ -1168,31 +1168,31 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" t="s">
         <v>25</v>
       </c>
-      <c r="B19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" t="s">
-        <v>0</v>
-      </c>
-      <c r="E19" t="s">
-        <v>15</v>
-      </c>
-      <c r="F19" t="s">
-        <v>18</v>
-      </c>
       <c r="G19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H19" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="I19" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="J19">
         <v>2</v>
@@ -1200,31 +1200,31 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D20" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E20" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F20" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="G20" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H20" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="I20" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="J20">
         <v>3</v>
@@ -1232,31 +1232,31 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E21" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="F21" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="G21" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H21" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="I21" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="J21">
         <v>3</v>
@@ -1264,31 +1264,31 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" t="s">
         <v>25</v>
       </c>
-      <c r="B22" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" t="s">
-        <v>0</v>
-      </c>
-      <c r="E22" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" t="s">
-        <v>18</v>
-      </c>
       <c r="G22" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H22" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I22" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="J22">
         <v>1</v>
@@ -1296,31 +1296,31 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D23" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E23" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="F23" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="G23" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H23" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I23" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="J23">
         <v>1</v>
@@ -1328,31 +1328,31 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D24" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E24" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="F24" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="G24" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H24" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I24" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="J24">
         <v>1</v>

</xml_diff>

<commit_message>
add loading code to animate a gif file.
</commit_message>
<xml_diff>
--- a/dataset_50.xlsx
+++ b/dataset_50.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Sepah\wall_recommender\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDEF8198-443B-48ED-B0B0-F537B6F0696D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4253DD05-D895-4EE4-89CF-A6518FBD7C1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20610" yWindow="3825" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="26">
   <si>
     <t>water_level</t>
   </si>
@@ -157,7 +157,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -189,12 +189,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" readingOrder="2"/>
@@ -211,6 +248,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -290,8 +330,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5469D414-C76D-475F-8DBF-B402E31C2529}" name="Table1" displayName="Table1" ref="A1:J24" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1" totalsRowBorderDxfId="0">
-  <autoFilter ref="A1:J24" xr:uid="{3666685D-B581-4997-AE6C-4CA1E08DE5ED}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5469D414-C76D-475F-8DBF-B402E31C2529}" name="Table1" displayName="Table1" ref="A1:J32" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1" totalsRowBorderDxfId="0">
+  <autoFilter ref="A1:J32" xr:uid="{3666685D-B581-4997-AE6C-4CA1E08DE5ED}"/>
   <tableColumns count="10">
     <tableColumn id="2" xr3:uid="{BACC7EB3-7AB7-4287-9974-A4729ADCEF86}" name="accessibilityes"/>
     <tableColumn id="3" xr3:uid="{599103BA-5FA5-434F-B4C2-0ACF492F0C9A}" name="defenosive"/>
@@ -571,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1358,6 +1398,678 @@
         <v>1</v>
       </c>
     </row>
+    <row r="25" spans="1:10">
+      <c r="A25" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" t="s">
+        <v>6</v>
+      </c>
+      <c r="F25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G25" t="s">
+        <v>22</v>
+      </c>
+      <c r="H25" t="s">
+        <v>24</v>
+      </c>
+      <c r="I25" t="s">
+        <v>6</v>
+      </c>
+      <c r="J25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" t="s">
+        <v>8</v>
+      </c>
+      <c r="G26" t="s">
+        <v>23</v>
+      </c>
+      <c r="H26" t="s">
+        <v>10</v>
+      </c>
+      <c r="I26" t="s">
+        <v>6</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" t="s">
+        <v>25</v>
+      </c>
+      <c r="G27" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" t="s">
+        <v>24</v>
+      </c>
+      <c r="I27" t="s">
+        <v>6</v>
+      </c>
+      <c r="J27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28" t="s">
+        <v>8</v>
+      </c>
+      <c r="G28" t="s">
+        <v>9</v>
+      </c>
+      <c r="H28" t="s">
+        <v>10</v>
+      </c>
+      <c r="I28" t="s">
+        <v>6</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" t="s">
+        <v>25</v>
+      </c>
+      <c r="G29" t="s">
+        <v>22</v>
+      </c>
+      <c r="H29" t="s">
+        <v>10</v>
+      </c>
+      <c r="I29" t="s">
+        <v>6</v>
+      </c>
+      <c r="J29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" t="s">
+        <v>8</v>
+      </c>
+      <c r="G30" t="s">
+        <v>23</v>
+      </c>
+      <c r="H30" t="s">
+        <v>10</v>
+      </c>
+      <c r="I30" t="s">
+        <v>7</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" t="s">
+        <v>20</v>
+      </c>
+      <c r="E31" t="s">
+        <v>6</v>
+      </c>
+      <c r="F31" t="s">
+        <v>25</v>
+      </c>
+      <c r="G31" t="s">
+        <v>22</v>
+      </c>
+      <c r="H31" t="s">
+        <v>10</v>
+      </c>
+      <c r="I31" t="s">
+        <v>6</v>
+      </c>
+      <c r="J31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" t="s">
+        <v>20</v>
+      </c>
+      <c r="E32" t="s">
+        <v>6</v>
+      </c>
+      <c r="F32" t="s">
+        <v>25</v>
+      </c>
+      <c r="G32" t="s">
+        <v>22</v>
+      </c>
+      <c r="H32" t="s">
+        <v>24</v>
+      </c>
+      <c r="I32" t="s">
+        <v>7</v>
+      </c>
+      <c r="J32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H33" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I33" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J33" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H34" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I34" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J34" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H35" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I35" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J35" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H36" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I36" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J36" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H37" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I37" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J37" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H38" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I38" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J38" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H39" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I39" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J39" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H40" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I40" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J40" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H41" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I41" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J41" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G42" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H42" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I42" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J42" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H43" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I43" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J43" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G44" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H44" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I44" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J44" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H45" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I45" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J45" s="8">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>